<commit_message>
Orbital User to MAGELLANO analysis
</commit_message>
<xml_diff>
--- a/Mars Orbits.xlsx
+++ b/Mars Orbits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lyle\Documents\GitHub\Telecomm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B490EBBB-4AAC-4F9E-9601-0A9F4D9EC13A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C76B7AF-8CD4-47BD-9A7D-C219155BD54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46D0ED4A-3E49-4B22-97B2-264D5A6B40FB}"/>
   </bookViews>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D3ED5C-3C54-4484-BB8E-7F90652302E5}">
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="34">
-        <v>18500</v>
+        <v>12000</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="C8" s="4">
         <f>C7+$C$4</f>
-        <v>21896</v>
+        <v>15396</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
@@ -933,7 +933,7 @@
       </c>
       <c r="C9" s="6">
         <f>$C$2/C$22*(1-C$20)</f>
-        <v>0.7516408419771452</v>
+        <v>1.6678613540976948</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>18</v>
@@ -943,7 +943,7 @@
       </c>
       <c r="G9" s="6">
         <f>$C$2/G$22*(1-G$20)</f>
-        <v>1.1758742082258424</v>
+        <v>1.8490955770571775</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>18</v>
@@ -965,7 +965,7 @@
       </c>
       <c r="C10" s="6">
         <f>SQRT(2*$C$2/C8)</f>
-        <v>1.9778643501642656</v>
+        <v>2.3587121471229149</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>18</v>
@@ -997,7 +997,7 @@
       </c>
       <c r="C11" s="6">
         <f>C10-C9</f>
-        <v>1.2262235081871204</v>
+        <v>0.69085079302522012</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>18</v>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="G11" s="6">
         <f>G10-G9</f>
-        <v>1.3527909548035419</v>
+        <v>0.67956958597220685</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>18</v>
@@ -1039,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="25">
-        <v>300</v>
+        <v>12000</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>7</v>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="G13" s="15">
         <f>C13</f>
-        <v>300</v>
+        <v>12000</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>7</v>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C14" s="9">
         <f>C13+$C$4</f>
-        <v>3696</v>
+        <v>15396</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="G14" s="9">
         <f>G13+$C$4</f>
-        <v>3696</v>
+        <v>15396</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>7</v>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="C15" s="6">
         <f>$C$2/C$22*(1+C$20)</f>
-        <v>4.4529025638342992</v>
+        <v>1.6678613540976948</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>18</v>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G15" s="6">
         <f>$C$2/G$22*(1+G$20)</f>
-        <v>4.2619077092514583</v>
+        <v>1.6088909034981782</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>18</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="C16" s="6">
         <f>SQRT(2*$C$2/C14)</f>
-        <v>4.814075682342839</v>
+        <v>2.3587121471229149</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="G16" s="6">
         <f>SQRT(2*$C$2/G14)</f>
-        <v>4.814075682342839</v>
+        <v>2.3587121471229149</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>18</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="C17" s="6">
         <f>C16-C15</f>
-        <v>0.36117311850853984</v>
+        <v>0.69085079302522012</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="G17" s="6">
         <f>G16-G15</f>
-        <v>0.55216797309138066</v>
+        <v>0.74982124362473668</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>18</v>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="C19" s="7">
         <f>(C8+C14)/2</f>
-        <v>12796</v>
+        <v>15396</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>7</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="G19" s="7">
         <f>(G8+G14)/2</f>
-        <v>8546</v>
+        <v>14396</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>7</v>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C20" s="10">
         <f>(C8-C14)/(C8+C14)</f>
-        <v>0.71115973741794314</v>
+        <v>0</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="3" t="s">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="G20" s="10">
         <f>(G8-G14)/(G8+G14)</f>
-        <v>0.5675169670021063</v>
+        <v>-6.9463739927757714E-2</v>
       </c>
       <c r="H20" s="5"/>
       <c r="J20" s="3" t="s">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="C21" s="11">
         <f>C19*(1-C20^2)</f>
-        <v>6324.4463894967166</v>
+        <v>15396</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>7</v>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="G21" s="11">
         <f>G19*(1-G20^2)</f>
-        <v>5793.5427100397837</v>
+        <v>14326.536260072242</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>7</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="C22" s="11">
         <f>SQRT(C21*$C$2)</f>
-        <v>16457.927875931568</v>
+        <v>25678.393407688105</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="G22" s="11">
         <f>SQRT(G21*$C$2)</f>
-        <v>15752.010893393384</v>
+        <v>24770.48435025795</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>17</v>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C23" s="11">
         <f>2*PI()*SQRT(C19^3/$C$2)</f>
-        <v>43946.806193124525</v>
+        <v>57999.977487139869</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>11</v>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="G23" s="11">
         <f>2*PI()*SQRT(G19^3/$C$2)</f>
-        <v>23986.136679442734</v>
+        <v>52441.937467826938</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>11</v>
@@ -1361,7 +1361,7 @@
       <c r="B24" s="39"/>
       <c r="C24" s="12">
         <f>C23/3600</f>
-        <v>12.207446164756812</v>
+        <v>16.111104857538852</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -1369,7 +1369,7 @@
       <c r="F24" s="39"/>
       <c r="G24" s="12">
         <f>G23/3600</f>
-        <v>6.6628157442896487</v>
+        <v>14.56720485217415</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>12</v>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="G26" s="19">
         <f>ABS(G15-C15)</f>
-        <v>0.19099485458284082</v>
+        <v>5.8970450599516555E-2</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>18</v>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="G27" s="22">
         <f>ABS(K9-G9)</f>
-        <v>0.612162075902422</v>
+        <v>6.10592929289131E-2</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>18</v>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="G28" s="24">
         <f>SUM(G26:G27)</f>
-        <v>0.80315693048526282</v>
+        <v>0.12002974352842966</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Included option for ECS to have a dumb-bob prism hanging down below
</commit_message>
<xml_diff>
--- a/Mars Orbits.xlsx
+++ b/Mars Orbits.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lyle\Documents\GitHub\Telecomm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C76B7AF-8CD4-47BD-9A7D-C219155BD54B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A320FF-EF0F-46F0-81B6-E4780AA8BA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46D0ED4A-3E49-4B22-97B2-264D5A6B40FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Mars-Mars" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Earth-Mars" sheetId="2" r:id="rId3"/>
-    <sheet name="Mars Capture" sheetId="3" r:id="rId4"/>
+    <sheet name="Mars Eclipse" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Earth-Mars" sheetId="2" r:id="rId4"/>
+    <sheet name="Mars Capture" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="64">
   <si>
     <t>r_Per</t>
   </si>
@@ -217,6 +218,18 @@
   </si>
   <si>
     <t>Propellant Mass</t>
+  </si>
+  <si>
+    <t>Orbit SMA</t>
+  </si>
+  <si>
+    <t>Circumference</t>
+  </si>
+  <si>
+    <t>Mars diam</t>
+  </si>
+  <si>
+    <t>Theta</t>
   </si>
 </sst>
 </file>
@@ -411,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -479,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,7 +810,7 @@
   <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +884,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="34">
-        <v>12000</v>
+        <v>7000</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -901,7 +915,7 @@
       </c>
       <c r="C8" s="4">
         <f>C7+$C$4</f>
-        <v>15396</v>
+        <v>10396</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
@@ -933,7 +947,7 @@
       </c>
       <c r="C9" s="6">
         <f>$C$2/C$22*(1-C$20)</f>
-        <v>1.6678613540976948</v>
+        <v>2.0296949052096318</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>18</v>
@@ -943,7 +957,7 @@
       </c>
       <c r="G9" s="6">
         <f>$C$2/G$22*(1-G$20)</f>
-        <v>1.8490955770571775</v>
+        <v>1.671510023371543</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>18</v>
@@ -965,7 +979,7 @@
       </c>
       <c r="C10" s="6">
         <f>SQRT(2*$C$2/C8)</f>
-        <v>2.3587121471229149</v>
+        <v>2.8704220624270347</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>18</v>
@@ -997,7 +1011,7 @@
       </c>
       <c r="C11" s="6">
         <f>C10-C9</f>
-        <v>0.69085079302522012</v>
+        <v>0.84072715721740288</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>18</v>
@@ -1007,7 +1021,7 @@
       </c>
       <c r="G11" s="6">
         <f>G10-G9</f>
-        <v>0.67956958597220685</v>
+        <v>0.8571551396578414</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>18</v>
@@ -1039,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="25">
-        <v>12000</v>
+        <v>7000</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>7</v>
@@ -1049,7 +1063,7 @@
       </c>
       <c r="G13" s="15">
         <f>C13</f>
-        <v>12000</v>
+        <v>7000</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>7</v>
@@ -1070,7 +1084,7 @@
       </c>
       <c r="C14" s="9">
         <f>C13+$C$4</f>
-        <v>15396</v>
+        <v>10396</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>
@@ -1080,7 +1094,7 @@
       </c>
       <c r="G14" s="9">
         <f>G13+$C$4</f>
-        <v>15396</v>
+        <v>10396</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>7</v>
@@ -1102,7 +1116,7 @@
       </c>
       <c r="C15" s="6">
         <f>$C$2/C$22*(1+C$20)</f>
-        <v>1.6678613540976948</v>
+        <v>2.0296949052096318</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>18</v>
@@ -1112,7 +1126,7 @@
       </c>
       <c r="G15" s="6">
         <f>$C$2/G$22*(1+G$20)</f>
-        <v>1.6088909034981782</v>
+        <v>2.1538618962182756</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>18</v>
@@ -1134,7 +1148,7 @@
       </c>
       <c r="C16" s="6">
         <f>SQRT(2*$C$2/C14)</f>
-        <v>2.3587121471229149</v>
+        <v>2.8704220624270347</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
@@ -1144,7 +1158,7 @@
       </c>
       <c r="G16" s="6">
         <f>SQRT(2*$C$2/G14)</f>
-        <v>2.3587121471229149</v>
+        <v>2.8704220624270347</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>18</v>
@@ -1166,7 +1180,7 @@
       </c>
       <c r="C17" s="6">
         <f>C16-C15</f>
-        <v>0.69085079302522012</v>
+        <v>0.84072715721740288</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -1176,7 +1190,7 @@
       </c>
       <c r="G17" s="6">
         <f>G16-G15</f>
-        <v>0.74982124362473668</v>
+        <v>0.71656016620875906</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>18</v>
@@ -1209,7 +1223,7 @@
       </c>
       <c r="C19" s="7">
         <f>(C8+C14)/2</f>
-        <v>15396</v>
+        <v>10396</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>7</v>
@@ -1219,7 +1233,7 @@
       </c>
       <c r="G19" s="7">
         <f>(G8+G14)/2</f>
-        <v>14396</v>
+        <v>11896</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>7</v>
@@ -1249,7 +1263,7 @@
       </c>
       <c r="G20" s="10">
         <f>(G8-G14)/(G8+G14)</f>
-        <v>-6.9463739927757714E-2</v>
+        <v>0.12609280430396771</v>
       </c>
       <c r="H20" s="5"/>
       <c r="J20" s="3" t="s">
@@ -1267,7 +1281,7 @@
       </c>
       <c r="C21" s="11">
         <f>C19*(1-C20^2)</f>
-        <v>15396</v>
+        <v>10396</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>7</v>
@@ -1277,7 +1291,7 @@
       </c>
       <c r="G21" s="11">
         <f>G19*(1-G20^2)</f>
-        <v>14326.536260072242</v>
+        <v>11706.860793544049</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>7</v>
@@ -1299,7 +1313,7 @@
       </c>
       <c r="C22" s="11">
         <f>SQRT(C21*$C$2)</f>
-        <v>25678.393407688105</v>
+        <v>21100.708234559334</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
@@ -1309,7 +1323,7 @@
       </c>
       <c r="G22" s="11">
         <f>SQRT(G21*$C$2)</f>
-        <v>24770.48435025795</v>
+        <v>22391.548273085195</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>17</v>
@@ -1331,7 +1345,7 @@
       </c>
       <c r="C23" s="11">
         <f>2*PI()*SQRT(C19^3/$C$2)</f>
-        <v>57999.977487139869</v>
+        <v>32182.17392465326</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>11</v>
@@ -1341,7 +1355,7 @@
       </c>
       <c r="G23" s="11">
         <f>2*PI()*SQRT(G19^3/$C$2)</f>
-        <v>52441.937467826938</v>
+        <v>39392.850206556221</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>11</v>
@@ -1361,7 +1375,7 @@
       <c r="B24" s="39"/>
       <c r="C24" s="12">
         <f>C23/3600</f>
-        <v>16.111104857538852</v>
+        <v>8.9394927568481268</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -1369,7 +1383,7 @@
       <c r="F24" s="39"/>
       <c r="G24" s="12">
         <f>G23/3600</f>
-        <v>14.56720485217415</v>
+        <v>10.942458390710062</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>12</v>
@@ -1390,7 +1404,7 @@
       </c>
       <c r="G26" s="19">
         <f>ABS(G15-C15)</f>
-        <v>5.8970450599516555E-2</v>
+        <v>0.12416699100864381</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>18</v>
@@ -1402,7 +1416,7 @@
       </c>
       <c r="G27" s="22">
         <f>ABS(K9-G9)</f>
-        <v>6.10592929289131E-2</v>
+        <v>0.11652626075672146</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>18</v>
@@ -1414,7 +1428,7 @@
       </c>
       <c r="G28" s="24">
         <f>SUM(G26:G27)</f>
-        <v>0.12002974352842966</v>
+        <v>0.24069325176536527</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>18</v>
@@ -1435,6 +1449,589 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F21BB8D-6EF4-4F00-A69B-DBCA8D941CB8}">
+  <dimension ref="C2:F36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <f>2*3390</f>
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="41">
+        <f>2*C5*PI()</f>
+        <v>31415.926535897932</v>
+      </c>
+      <c r="E5" s="29">
+        <f>2*ASIN($D$2/(2*C5))</f>
+        <v>1.4900766984267722</v>
+      </c>
+      <c r="F5">
+        <f>E5/(2*PI())</f>
+        <v>0.23715307214067222</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>5500</v>
+      </c>
+      <c r="D6" s="41">
+        <f t="shared" ref="D6:D36" si="0">2*C6*PI()</f>
+        <v>34557.519189487721</v>
+      </c>
+      <c r="E6" s="29">
+        <f t="shared" ref="E6:E29" si="1">2*ASIN($D$2/(2*C6))</f>
+        <v>1.3282329628029259</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F36" si="2">E6/(2*PI())</f>
+        <v>0.21139484160767921</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>6000</v>
+      </c>
+      <c r="D7" s="41">
+        <f t="shared" si="0"/>
+        <v>37699.111843077517</v>
+      </c>
+      <c r="E7" s="29">
+        <f t="shared" si="1"/>
+        <v>1.2008665071610467</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.19112384060817952</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>6500</v>
+      </c>
+      <c r="D8" s="41">
+        <f t="shared" si="0"/>
+        <v>40840.704496667313</v>
+      </c>
+      <c r="E8" s="29">
+        <f t="shared" si="1"/>
+        <v>1.0973061335537559</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.17464169524013573</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>7000</v>
+      </c>
+      <c r="D9" s="41">
+        <f t="shared" si="0"/>
+        <v>43982.297150257102</v>
+      </c>
+      <c r="E9" s="29">
+        <f t="shared" si="1"/>
+        <v>1.0110931448898759</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.1609204719355537</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>7500</v>
+      </c>
+      <c r="D10" s="41">
+        <f t="shared" si="0"/>
+        <v>47123.889803846898</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" si="1"/>
+        <v>0.93801235220684875</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.14928930253497591</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>8000</v>
+      </c>
+      <c r="D11" s="41">
+        <f t="shared" si="0"/>
+        <v>50265.482457436687</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="1"/>
+        <v>0.87516282421328206</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0.13928648948380731</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>8500</v>
+      </c>
+      <c r="D12" s="41">
+        <f t="shared" si="0"/>
+        <v>53407.075111026483</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="1"/>
+        <v>0.82046714085441064</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>0.1305814011114538</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>9000</v>
+      </c>
+      <c r="D13" s="41">
+        <f t="shared" si="0"/>
+        <v>56548.667764616279</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="1"/>
+        <v>0.77239059202228444</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0.12292978071802203</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>9500</v>
+      </c>
+      <c r="D14" s="41">
+        <f t="shared" si="0"/>
+        <v>59690.260418206068</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="1"/>
+        <v>0.72977050821628342</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0.11614658370530613</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>10000</v>
+      </c>
+      <c r="D15" s="41">
+        <f t="shared" si="0"/>
+        <v>62831.853071795864</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="1"/>
+        <v>0.69170750624173893</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.1100886687921408</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>10500</v>
+      </c>
+      <c r="D16" s="41">
+        <f t="shared" si="0"/>
+        <v>65973.445725385653</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="1"/>
+        <v>0.65749349196079299</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0.10464333929631156</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>11000</v>
+      </c>
+      <c r="D17" s="41">
+        <f t="shared" si="0"/>
+        <v>69115.038378975441</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.6265624685501201</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>9.9720514025611828E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>11500</v>
+      </c>
+      <c r="D18" s="41">
+        <f t="shared" si="0"/>
+        <v>72256.631032565245</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="1"/>
+        <v>0.59845602049744184</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>9.5247233885272509E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>12000</v>
+      </c>
+      <c r="D19" s="41">
+        <f t="shared" si="0"/>
+        <v>75398.223686155034</v>
+      </c>
+      <c r="E19" s="29">
+        <f t="shared" si="1"/>
+        <v>0.57279853714194451</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>9.1163718581947079E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>12500</v>
+      </c>
+      <c r="D20" s="41">
+        <f t="shared" si="0"/>
+        <v>78539.816339744822</v>
+      </c>
+      <c r="E20" s="29">
+        <f t="shared" si="1"/>
+        <v>0.54927907265337028</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>8.7420479549716198E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>13000</v>
+      </c>
+      <c r="D21" s="41">
+        <f t="shared" si="0"/>
+        <v>81681.408993334626</v>
+      </c>
+      <c r="E21" s="29">
+        <f t="shared" si="1"/>
+        <v>0.52763783270931575</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>8.3976169237982137E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>13500</v>
+      </c>
+      <c r="D22" s="41">
+        <f t="shared" si="0"/>
+        <v>84823.001646924415</v>
+      </c>
+      <c r="E22" s="29">
+        <f t="shared" si="1"/>
+        <v>0.50765595214619785</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>8.0795954174090065E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>14000</v>
+      </c>
+      <c r="D23" s="41">
+        <f t="shared" si="0"/>
+        <v>87964.594300514203</v>
+      </c>
+      <c r="E23" s="29">
+        <f t="shared" si="1"/>
+        <v>0.48914765544896099</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>7.7850267266513423E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>14500</v>
+      </c>
+      <c r="D24" s="41">
+        <f t="shared" si="0"/>
+        <v>91106.186954104007</v>
+      </c>
+      <c r="E24" s="29">
+        <f t="shared" si="1"/>
+        <v>0.47195417012110447</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>7.5113839087607076E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>15000</v>
+      </c>
+      <c r="D25" s="41">
+        <f t="shared" si="0"/>
+        <v>94247.779607693796</v>
+      </c>
+      <c r="E25" s="29">
+        <f t="shared" si="1"/>
+        <v>0.45593894803327445</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>7.2564937327614418E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>15500</v>
+      </c>
+      <c r="D26" s="41">
+        <f t="shared" si="0"/>
+        <v>97389.372261283585</v>
+      </c>
+      <c r="E26" s="29">
+        <f t="shared" si="1"/>
+        <v>0.44098387543539286</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>7.0184763599363417E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>16000</v>
+      </c>
+      <c r="D27" s="41">
+        <f t="shared" si="0"/>
+        <v>100530.96491487337</v>
+      </c>
+      <c r="E27" s="29">
+        <f t="shared" si="1"/>
+        <v>0.42698623908641925</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>6.7956970582821477E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>16500</v>
+      </c>
+      <c r="D28" s="41">
+        <f t="shared" si="0"/>
+        <v>103672.55756846318</v>
+      </c>
+      <c r="E28" s="29">
+        <f t="shared" si="1"/>
+        <v>0.41385627688535714</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>6.5867272195912693E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>17000</v>
+      </c>
+      <c r="D29" s="41">
+        <f t="shared" si="0"/>
+        <v>106814.15022205297</v>
+      </c>
+      <c r="E29" s="29">
+        <f t="shared" si="1"/>
+        <v>0.4015151848076231</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>6.3903126388589096E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>17500</v>
+      </c>
+      <c r="D30" s="41">
+        <f t="shared" si="0"/>
+        <v>109955.74287564275</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" ref="E30:E36" si="3">2*ASIN($D$2/(2*C30))</f>
+        <v>0.38989348331385315</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>6.2053475148717147E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>18000</v>
+      </c>
+      <c r="D31" s="41">
+        <f t="shared" si="0"/>
+        <v>113097.33552923256</v>
+      </c>
+      <c r="E31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.37892966933403399</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>6.0308529958688899E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>18500</v>
+      </c>
+      <c r="D32" s="41">
+        <f t="shared" si="0"/>
+        <v>116238.92818282235</v>
+      </c>
+      <c r="E32" s="29">
+        <f t="shared" si="3"/>
+        <v>0.36856909689534179</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>5.8659593641809379E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>19000</v>
+      </c>
+      <c r="D33" s="41">
+        <f t="shared" si="0"/>
+        <v>119380.52083641214</v>
+      </c>
+      <c r="E33" s="29">
+        <f t="shared" si="3"/>
+        <v>0.35876304214450988</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>5.7098911555984719E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>19500</v>
+      </c>
+      <c r="D34" s="41">
+        <f t="shared" si="0"/>
+        <v>122522.11349000194</v>
+      </c>
+      <c r="E34" s="29">
+        <f t="shared" si="3"/>
+        <v>0.34946791808956579</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>5.5619546615987989E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>20000</v>
+      </c>
+      <c r="D35" s="41">
+        <f t="shared" si="0"/>
+        <v>125663.70614359173</v>
+      </c>
+      <c r="E35" s="29">
+        <f t="shared" si="3"/>
+        <v>0.34064461167946047</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>5.4215273786405317E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>20500</v>
+      </c>
+      <c r="D36" s="41">
+        <f t="shared" si="0"/>
+        <v>128805.29879718152</v>
+      </c>
+      <c r="E36" s="29">
+        <f t="shared" si="3"/>
+        <v>0.33225792144411248</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>5.2880490579269156E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2470E4B0-A537-4156-B81A-3D2EB3DBBDEC}">
   <dimension ref="C2:G14"/>
   <sheetViews>
@@ -1485,7 +2082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0737E035-10CF-415D-9B82-EC76F9BAA130}">
   <dimension ref="B1:O22"/>
   <sheetViews>
@@ -1944,7 +2541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABCDF85-BE54-4F5B-B70F-7758956758A9}">
   <dimension ref="B2:P16"/>
   <sheetViews>

</xml_diff>